<commit_message>
updating sample configuration and rules; new sample configuration to process licenses.xml from a single maven project
</commit_message>
<xml_diff>
--- a/src/main/resources/samples/Solicitor_Output_Template_Sample.xlsx
+++ b/src/main/resources/samples/Solicitor_Output_Template_Sample.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7572AFE1-8706-4D04-98B8-5D63D9144780}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D384946-32F9-49D0-8037-BB90D4AD591D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Masterdata" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>#ENGAGEMENT#$engagementName$</t>
   </si>
@@ -176,12 +176,6 @@
 Normalized License</t>
   </si>
   <si>
-    <t>License Text</t>
-  </si>
-  <si>
-    <t>$effectiveNormalizedLicenseContent$</t>
-  </si>
-  <si>
     <t>Normalized
 License Type</t>
   </si>
@@ -194,9 +188,6 @@
   </si>
   <si>
     <t>$effectiveNormalizedLicenseType$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Copyright (of this XLS template) 2019 by Capgemini SE, SPDX-License-Identifier: Apache-2.0; </t>
   </si>
   <si>
     <t xml:space="preserve">Copyright (of the XLS template) 2019 by Capgemini SE, SPDX-License-Identifier: Apache-2.0; </t>
@@ -647,7 +638,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
@@ -720,7 +711,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -731,10 +722,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{613F3CEC-3E20-4A64-8FE7-D162064F8323}">
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="S1" sqref="S1:S1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -755,10 +746,9 @@
     <col min="16" max="16" width="29.5703125" style="5" customWidth="1"/>
     <col min="17" max="17" width="17.7109375" style="9" customWidth="1"/>
     <col min="18" max="18" width="19.5703125" style="9" customWidth="1"/>
-    <col min="19" max="19" width="79.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>41</v>
       </c>
@@ -781,7 +771,7 @@
         <v>44</v>
       </c>
       <c r="H1" s="19" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I1" s="14" t="s">
         <v>19</v>
@@ -790,7 +780,7 @@
         <v>20</v>
       </c>
       <c r="K1" s="15" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="L1" s="15" t="s">
         <v>47</v>
@@ -813,11 +803,8 @@
       <c r="R1" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="S1" s="4" t="s">
-        <v>48</v>
-      </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>25</v>
       </c>
@@ -840,7 +827,7 @@
         <v>33</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I2" s="6" t="s">
         <v>31</v>
@@ -849,7 +836,7 @@
         <v>32</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="L2" s="7" t="s">
         <v>34</v>
@@ -871,9 +858,6 @@
       </c>
       <c r="R2" s="9" t="s">
         <v>40</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating sample configuration and rules; new sample configuration to process licenses.xml from a single maven project (#3)
</commit_message>
<xml_diff>
--- a/src/main/resources/samples/Solicitor_Output_Template_Sample.xlsx
+++ b/src/main/resources/samples/Solicitor_Output_Template_Sample.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7572AFE1-8706-4D04-98B8-5D63D9144780}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D384946-32F9-49D0-8037-BB90D4AD591D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Masterdata" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>#ENGAGEMENT#$engagementName$</t>
   </si>
@@ -176,12 +176,6 @@
 Normalized License</t>
   </si>
   <si>
-    <t>License Text</t>
-  </si>
-  <si>
-    <t>$effectiveNormalizedLicenseContent$</t>
-  </si>
-  <si>
     <t>Normalized
 License Type</t>
   </si>
@@ -194,9 +188,6 @@
   </si>
   <si>
     <t>$effectiveNormalizedLicenseType$</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Copyright (of this XLS template) 2019 by Capgemini SE, SPDX-License-Identifier: Apache-2.0; </t>
   </si>
   <si>
     <t xml:space="preserve">Copyright (of the XLS template) 2019 by Capgemini SE, SPDX-License-Identifier: Apache-2.0; </t>
@@ -647,7 +638,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
@@ -720,7 +711,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -731,10 +722,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{613F3CEC-3E20-4A64-8FE7-D162064F8323}">
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="S1" sqref="S1:S1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -755,10 +746,9 @@
     <col min="16" max="16" width="29.5703125" style="5" customWidth="1"/>
     <col min="17" max="17" width="17.7109375" style="9" customWidth="1"/>
     <col min="18" max="18" width="19.5703125" style="9" customWidth="1"/>
-    <col min="19" max="19" width="79.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>41</v>
       </c>
@@ -781,7 +771,7 @@
         <v>44</v>
       </c>
       <c r="H1" s="19" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I1" s="14" t="s">
         <v>19</v>
@@ -790,7 +780,7 @@
         <v>20</v>
       </c>
       <c r="K1" s="15" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="L1" s="15" t="s">
         <v>47</v>
@@ -813,11 +803,8 @@
       <c r="R1" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="S1" s="4" t="s">
-        <v>48</v>
-      </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>25</v>
       </c>
@@ -840,7 +827,7 @@
         <v>33</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="I2" s="6" t="s">
         <v>31</v>
@@ -849,7 +836,7 @@
         <v>32</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="L2" s="7" t="s">
         <v>34</v>
@@ -871,9 +858,6 @@
       </c>
       <c r="R2" s="9" t="s">
         <v>40</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change copyright/licensing boilerplate to conform to devonfw standards
</commit_message>
<xml_diff>
--- a/src/main/resources/samples/Solicitor_Output_Template_Sample.xlsx
+++ b/src/main/resources/samples/Solicitor_Output_Template_Sample.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D384946-32F9-49D0-8037-BB90D4AD591D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F174844-3631-4F3D-A242-0EB929B8EB5C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Masterdata" sheetId="1" r:id="rId1"/>
@@ -190,7 +190,7 @@
     <t>$effectiveNormalizedLicenseType$</t>
   </si>
   <si>
-    <t xml:space="preserve">Copyright (of the XLS template) 2019 by Capgemini SE, SPDX-License-Identifier: Apache-2.0; </t>
+    <t xml:space="preserve">The template file for creating this XLS is licensed as follows: SPDX-License-Identifier: Apache-2.0; </t>
   </si>
 </sst>
 </file>
@@ -638,7 +638,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
@@ -724,7 +724,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{613F3CEC-3E20-4A64-8FE7-D162064F8323}">
   <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+    <sheetView topLeftCell="L1" workbookViewId="0">
       <selection activeCell="S1" sqref="S1:S1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Create log of import activities and rule executions in field "trace" of NormalizedLicense. This closes #14.
</commit_message>
<xml_diff>
--- a/src/main/resources/samples/Solicitor_Output_Template_Sample.xlsx
+++ b/src/main/resources/samples/Solicitor_Output_Template_Sample.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F174844-3631-4F3D-A242-0EB929B8EB5C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48DE3CED-EDF4-46FC-8B23-EF03FF63A5DA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Masterdata" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
   <si>
     <t>#ENGAGEMENT#$engagementName$</t>
   </si>
@@ -191,6 +191,12 @@
   </si>
   <si>
     <t xml:space="preserve">The template file for creating this XLS is licensed as follows: SPDX-License-Identifier: Apache-2.0; </t>
+  </si>
+  <si>
+    <t>$trace$</t>
+  </si>
+  <si>
+    <t>Trace</t>
   </si>
 </sst>
 </file>
@@ -229,7 +235,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -311,6 +317,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39994506668294322"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -327,7 +339,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -354,6 +366,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -638,7 +653,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
@@ -722,10 +737,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{613F3CEC-3E20-4A64-8FE7-D162064F8323}">
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="S1" sqref="S1:S1048576"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="V18" sqref="V18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -746,9 +761,10 @@
     <col min="16" max="16" width="29.5703125" style="5" customWidth="1"/>
     <col min="17" max="17" width="17.7109375" style="9" customWidth="1"/>
     <col min="18" max="18" width="19.5703125" style="9" customWidth="1"/>
+    <col min="19" max="19" width="19.5703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>41</v>
       </c>
@@ -803,8 +819,11 @@
       <c r="R1" s="18" t="s">
         <v>24</v>
       </c>
+      <c r="S1" s="20" t="s">
+        <v>54</v>
+      </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>25</v>
       </c>
@@ -858,9 +877,13 @@
       </c>
       <c r="R2" s="9" t="s">
         <v>40</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Implemented Functionality to report diffs between two different execution results: - Drop and recreate reporting tables for every writer - Store engagement only as local variable - Introduce ModelRoot as root element for the data model - added command line option "d/diff" - Introduction of DataTableField as container for data in a table which allows to store old and new value - Central diff functionality implemented - Sample to show diff results in Velocity Reports - Diff for XLS: insert comment (note) for new lines or changed fields - Added Version and Build-Info to ModelRoot - Bounced version number
</commit_message>
<xml_diff>
--- a/src/main/resources/samples/Solicitor_Output_Template_Sample.xlsx
+++ b/src/main/resources/samples/Solicitor_Output_Template_Sample.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48DE3CED-EDF4-46FC-8B23-EF03FF63A5DA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{262AEFEE-5047-4560-B30D-E2F70C0BD291}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Masterdata" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
     <t>#ENGAGEMENT#$engagementName$</t>
   </si>
@@ -197,6 +197,30 @@
   </si>
   <si>
     <t>Trace</t>
+  </si>
+  <si>
+    <t>Solicitor Version:</t>
+  </si>
+  <si>
+    <t>Solicitor processing at:</t>
+  </si>
+  <si>
+    <t>Solicitor Buildnumber:</t>
+  </si>
+  <si>
+    <t>Solicitor Builddate:</t>
+  </si>
+  <si>
+    <t>#MODELROOT#$solicitorVersion$</t>
+  </si>
+  <si>
+    <t>#MODELROOT#$executionTime$</t>
+  </si>
+  <si>
+    <t>#MODELROOT#$solicitorGitHash$</t>
+  </si>
+  <si>
+    <t>#MODELROOT#$solicitorBuilddate$</t>
   </si>
 </sst>
 </file>
@@ -339,10 +363,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
@@ -371,6 +394,8 @@
     <xf numFmtId="0" fontId="3" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -651,10 +676,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -668,64 +693,97 @@
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:6" s="20" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="20" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="21" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+    <row r="3" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D9" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F9" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>52</v>
       </c>
     </row>
@@ -739,87 +797,87 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{613F3CEC-3E20-4A64-8FE7-D162064F8323}">
   <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+    <sheetView topLeftCell="L1" workbookViewId="0">
       <selection activeCell="V18" sqref="V18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="32.7109375" style="5" customWidth="1"/>
-    <col min="3" max="3" width="26.140625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" style="5" customWidth="1"/>
-    <col min="5" max="5" width="26" style="5" customWidth="1"/>
-    <col min="6" max="6" width="24.7109375" style="5" customWidth="1"/>
-    <col min="7" max="7" width="17.42578125" style="5" customWidth="1"/>
-    <col min="8" max="9" width="18.5703125" style="6" customWidth="1"/>
-    <col min="10" max="10" width="23.140625" style="6" customWidth="1"/>
-    <col min="11" max="12" width="28.7109375" style="7" customWidth="1"/>
-    <col min="13" max="13" width="31.5703125" style="7" customWidth="1"/>
-    <col min="14" max="14" width="20.42578125" style="8" customWidth="1"/>
-    <col min="15" max="15" width="20.140625" style="8" customWidth="1"/>
-    <col min="16" max="16" width="29.5703125" style="5" customWidth="1"/>
-    <col min="17" max="17" width="17.7109375" style="9" customWidth="1"/>
-    <col min="18" max="18" width="19.5703125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="32.7109375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="26.140625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="26" style="4" customWidth="1"/>
+    <col min="6" max="6" width="24.7109375" style="4" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" style="4" customWidth="1"/>
+    <col min="8" max="9" width="18.5703125" style="5" customWidth="1"/>
+    <col min="10" max="10" width="23.140625" style="5" customWidth="1"/>
+    <col min="11" max="12" width="28.7109375" style="6" customWidth="1"/>
+    <col min="13" max="13" width="31.5703125" style="6" customWidth="1"/>
+    <col min="14" max="14" width="20.42578125" style="7" customWidth="1"/>
+    <col min="15" max="15" width="20.140625" style="7" customWidth="1"/>
+    <col min="16" max="16" width="29.5703125" style="4" customWidth="1"/>
+    <col min="17" max="17" width="17.7109375" style="8" customWidth="1"/>
+    <col min="18" max="18" width="19.5703125" style="8" customWidth="1"/>
     <col min="19" max="19" width="19.5703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:19" s="9" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="H1" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="I1" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="J1" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="15" t="s">
+      <c r="K1" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="L1" s="15" t="s">
+      <c r="L1" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="M1" s="16" t="s">
+      <c r="M1" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="17" t="s">
+      <c r="N1" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="O1" s="17" t="s">
+      <c r="O1" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="P1" s="13" t="s">
+      <c r="P1" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="Q1" s="18" t="s">
+      <c r="Q1" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="R1" s="18" t="s">
+      <c r="R1" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="S1" s="20" t="s">
+      <c r="S1" s="19" t="s">
         <v>54</v>
       </c>
     </row>
@@ -827,55 +885,55 @@
       <c r="A2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="J2" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="K2" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="L2" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="M2" s="7" t="s">
+      <c r="M2" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="N2" s="8" t="s">
+      <c r="N2" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="O2" s="8" t="s">
+      <c r="O2" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="P2" s="5" t="s">
+      <c r="P2" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="Q2" s="9" t="s">
+      <c r="Q2" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="R2" s="9" t="s">
+      <c r="R2" s="8" t="s">
         <v>40</v>
       </c>
       <c r="S2" s="1" t="s">

</xml_diff>

<commit_message>
Implemented Functionality to report diffs between two different execution results: (#30)
- Drop and recreate reporting tables for every writer
- Store engagement only as local variable
- Introduce ModelRoot as root element for the data model
- added command line option "d/diff"
- Introduction of DataTableField as container for data in a table which allows to store old and new value
- Central diff functionality implemented
- Sample to show diff results in Velocity Reports
- Diff for XLS: insert comment (note) for new lines or changed fields
- Added Version and Build-Info to ModelRoot
- Bounced version number
</commit_message>
<xml_diff>
--- a/src/main/resources/samples/Solicitor_Output_Template_Sample.xlsx
+++ b/src/main/resources/samples/Solicitor_Output_Template_Sample.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48DE3CED-EDF4-46FC-8B23-EF03FF63A5DA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{262AEFEE-5047-4560-B30D-E2F70C0BD291}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Masterdata" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
     <t>#ENGAGEMENT#$engagementName$</t>
   </si>
@@ -197,6 +197,30 @@
   </si>
   <si>
     <t>Trace</t>
+  </si>
+  <si>
+    <t>Solicitor Version:</t>
+  </si>
+  <si>
+    <t>Solicitor processing at:</t>
+  </si>
+  <si>
+    <t>Solicitor Buildnumber:</t>
+  </si>
+  <si>
+    <t>Solicitor Builddate:</t>
+  </si>
+  <si>
+    <t>#MODELROOT#$solicitorVersion$</t>
+  </si>
+  <si>
+    <t>#MODELROOT#$executionTime$</t>
+  </si>
+  <si>
+    <t>#MODELROOT#$solicitorGitHash$</t>
+  </si>
+  <si>
+    <t>#MODELROOT#$solicitorBuilddate$</t>
   </si>
 </sst>
 </file>
@@ -339,10 +363,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
@@ -371,6 +394,8 @@
     <xf numFmtId="0" fontId="3" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -651,10 +676,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -668,64 +693,97 @@
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:6" s="20" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="20" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="21" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+    <row r="3" spans="1:6" s="21" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D9" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E9" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F9" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>52</v>
       </c>
     </row>
@@ -739,87 +797,87 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{613F3CEC-3E20-4A64-8FE7-D162064F8323}">
   <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+    <sheetView topLeftCell="L1" workbookViewId="0">
       <selection activeCell="V18" sqref="V18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="32.7109375" style="5" customWidth="1"/>
-    <col min="3" max="3" width="26.140625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" style="5" customWidth="1"/>
-    <col min="5" max="5" width="26" style="5" customWidth="1"/>
-    <col min="6" max="6" width="24.7109375" style="5" customWidth="1"/>
-    <col min="7" max="7" width="17.42578125" style="5" customWidth="1"/>
-    <col min="8" max="9" width="18.5703125" style="6" customWidth="1"/>
-    <col min="10" max="10" width="23.140625" style="6" customWidth="1"/>
-    <col min="11" max="12" width="28.7109375" style="7" customWidth="1"/>
-    <col min="13" max="13" width="31.5703125" style="7" customWidth="1"/>
-    <col min="14" max="14" width="20.42578125" style="8" customWidth="1"/>
-    <col min="15" max="15" width="20.140625" style="8" customWidth="1"/>
-    <col min="16" max="16" width="29.5703125" style="5" customWidth="1"/>
-    <col min="17" max="17" width="17.7109375" style="9" customWidth="1"/>
-    <col min="18" max="18" width="19.5703125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="32.7109375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="26.140625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="26" style="4" customWidth="1"/>
+    <col min="6" max="6" width="24.7109375" style="4" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" style="4" customWidth="1"/>
+    <col min="8" max="9" width="18.5703125" style="5" customWidth="1"/>
+    <col min="10" max="10" width="23.140625" style="5" customWidth="1"/>
+    <col min="11" max="12" width="28.7109375" style="6" customWidth="1"/>
+    <col min="13" max="13" width="31.5703125" style="6" customWidth="1"/>
+    <col min="14" max="14" width="20.42578125" style="7" customWidth="1"/>
+    <col min="15" max="15" width="20.140625" style="7" customWidth="1"/>
+    <col min="16" max="16" width="29.5703125" style="4" customWidth="1"/>
+    <col min="17" max="17" width="17.7109375" style="8" customWidth="1"/>
+    <col min="18" max="18" width="19.5703125" style="8" customWidth="1"/>
     <col min="19" max="19" width="19.5703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:19" s="9" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="G1" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="H1" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="I1" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="J1" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="15" t="s">
+      <c r="K1" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="L1" s="15" t="s">
+      <c r="L1" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="M1" s="16" t="s">
+      <c r="M1" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="17" t="s">
+      <c r="N1" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="O1" s="17" t="s">
+      <c r="O1" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="P1" s="13" t="s">
+      <c r="P1" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="Q1" s="18" t="s">
+      <c r="Q1" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="R1" s="18" t="s">
+      <c r="R1" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="S1" s="20" t="s">
+      <c r="S1" s="19" t="s">
         <v>54</v>
       </c>
     </row>
@@ -827,55 +885,55 @@
       <c r="A2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="J2" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="K2" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="L2" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="M2" s="7" t="s">
+      <c r="M2" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="N2" s="8" t="s">
+      <c r="N2" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="O2" s="8" t="s">
+      <c r="O2" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="P2" s="5" t="s">
+      <c r="P2" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="Q2" s="9" t="s">
+      <c r="Q2" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="R2" s="9" t="s">
+      <c r="R2" s="8" t="s">
         <v>40</v>
       </c>
       <c r="S2" s="1" t="s">

</xml_diff>